<commit_message>
corregidos ciertos errores en kettle y en el excel 2004 ahora ya va bien la subida de multiples temporadas
</commit_message>
<xml_diff>
--- a/Excels/data/2004.xlsx
+++ b/Excels/data/2004.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{866412B8-0272-4F74-AE6A-DBF9B600888A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73EE76A4-4622-4F47-988E-650D4EFDD700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="1" activeTab="4" xr2:uid="{5FACFDE8-0E5D-450C-9997-A9F216FA1A6F}"/>
   </bookViews>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="235">
   <si>
     <t>Round</t>
   </si>
@@ -787,9 +787,6 @@
   </si>
   <si>
     <t>33</t>
-  </si>
-  <si>
-    <t>Source:</t>
   </si>
   <si>
     <t>Columna1</t>
@@ -927,13 +924,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1521,13 +1517,13 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1535,13 +1531,13 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1549,13 +1545,13 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1563,13 +1559,13 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1577,13 +1573,13 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1591,13 +1587,13 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1605,13 +1601,13 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1619,13 +1615,13 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1633,13 +1629,13 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1647,13 +1643,13 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1661,13 +1657,13 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1675,13 +1671,13 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1689,13 +1685,13 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1703,13 +1699,13 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1717,13 +1713,13 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1731,13 +1727,13 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1753,7 +1749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DCEEADA-21DE-4E09-A46D-C942026BBB0D}">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -3592,10 +3588,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79ED2529-CCA3-4F4F-A698-BE65E13E91F5}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3633,854 +3629,831 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>161</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>162</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>163</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>129</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>128</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>161</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>162</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>165</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>161</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>162</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>166</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>150</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>161</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>162</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>168</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>126</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>170</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>170</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>162</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>171</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>101</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>172</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>162</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>108</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>172</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>162</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>173</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>122</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>135</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>134</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>174</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>175</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>151</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>135</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>134</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>134</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>174</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>177</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" t="s">
         <v>145</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>135</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>134</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>174</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>165</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" t="s">
         <v>133</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>135</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>134</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>174</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>180</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" t="s">
         <v>153</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>135</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>134</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>174</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>181</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" t="s">
         <v>142</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>183</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>162</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" t="s">
         <v>90</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>183</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>162</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>184</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>155</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>183</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>162</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>186</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" t="s">
         <v>154</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>183</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>162</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>107</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>183</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>162</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>187</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" t="s">
         <v>94</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>183</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>162</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>83</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" t="s">
         <v>86</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>183</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>188</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>84</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" t="s">
         <v>96</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>106</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>189</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>188</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>190</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" t="s">
         <v>104</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>105</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>189</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>188</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>191</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" t="s">
         <v>117</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>139</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>192</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>174</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>193</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" t="s">
         <v>144</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>140</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>139</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>192</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>174</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>118</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" t="s">
         <v>138</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>196</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>131</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>197</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>174</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>93</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" t="s">
         <v>130</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>196</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>197</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>174</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>198</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" t="s">
         <v>148</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>196</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>131</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>197</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>174</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>200</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" t="s">
         <v>141</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>121</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>120</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>202</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>188</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>98</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" t="s">
         <v>125</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>121</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>120</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>202</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>188</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>204</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" t="s">
         <v>137</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>121</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>202</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>188</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>206</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" t="s">
         <v>152</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>121</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>120</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>202</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>188</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>147</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" t="s">
         <v>119</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>121</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>120</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>202</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>188</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>206</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" t="s">
         <v>152</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>210</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>162</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>85</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" t="s">
         <v>99</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>210</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>162</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>211</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" t="s">
         <v>73</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>112</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>210</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" t="s">
         <v>162</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" t="s">
         <v>114</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G36" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>210</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" t="s">
         <v>162</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>212</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" t="s">
         <v>111</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -4495,7 +4468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34FD487F-3DE1-4D7E-AC38-49F580DAF036}">
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:Z1"/>
     </sheetView>
   </sheetViews>
@@ -4506,7 +4479,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -4585,1544 +4558,1544 @@
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="O2" s="4" t="s">
+      <c r="N2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="R2" s="3"/>
+      <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="H3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="R3" s="2"/>
+      <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="N4" s="4" t="s">
+      <c r="L4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="R4" s="3"/>
+      <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H5" s="5" t="s">
+      <c r="F5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="L5" s="5" t="s">
+      <c r="K5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="Q5" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="R5" s="2"/>
+      <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="M6" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="N6" s="4" t="s">
+      <c r="M6" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O6" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="P6" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="Q6" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="R6" s="3"/>
+      <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="E7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="P7" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="Q7" s="5" t="s">
+      <c r="Q7" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="R7" s="2"/>
+      <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="E8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="J8" s="4" t="s">
+      <c r="I8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="N8" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="O8" s="4" t="s">
+      <c r="N8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O8" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="Q8" s="4" t="s">
+      <c r="Q8" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="R8" s="3"/>
+      <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="E9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="K9" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="N9" s="5" t="s">
+      <c r="K9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="N9" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="O9" s="5" t="s">
+      <c r="O9" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="P9" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q9" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="R9" s="2"/>
+      <c r="Q9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" s="4" t="s">
+      <c r="I10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="M10" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="O10" s="4" t="s">
+      <c r="M10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="P10" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="Q10" s="4" t="s">
+      <c r="Q10" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="R10" s="3"/>
+      <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="5" t="s">
+      <c r="D11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H11" s="5" t="s">
+      <c r="G11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L11" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="M11" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="N11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="O11" s="5" t="s">
+      <c r="N11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O11" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="P11" s="5" t="s">
+      <c r="P11" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="Q11" s="5" t="s">
+      <c r="Q11" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="R11" s="2"/>
+      <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="B12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="M12" s="4" t="s">
+      <c r="K12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="N12" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O12" s="4" t="s">
+      <c r="O12" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="P12" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="Q12" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="R12" s="3"/>
+      <c r="Q12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="I13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="M13" s="5" t="s">
+      <c r="L13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M13" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="N13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="R13" s="2"/>
+      <c r="N13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="D14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="K14" s="4" t="s">
+      <c r="I14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="M14" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="N14" s="4" t="s">
+      <c r="M14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N14" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="P14" s="4" t="s">
+      <c r="P14" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="Q14" s="4" t="s">
+      <c r="Q14" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="R14" s="3"/>
+      <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="C15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J15" s="5" t="s">
+      <c r="F15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="K15" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="L15" s="5" t="s">
+      <c r="K15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="M15" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="N15" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="O15" s="5" t="s">
+      <c r="M15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O15" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="P15" s="5" t="s">
+      <c r="P15" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="Q15" s="5" t="s">
+      <c r="Q15" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="R15" s="2"/>
+      <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="D16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="N16" s="4" t="s">
+      <c r="N16" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="O16" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="P16" s="4" t="s">
+      <c r="O16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="P16" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="Q16" s="4" t="s">
+      <c r="Q16" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="R16" s="3"/>
+      <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="D17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="K17" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="L17" s="5" t="s">
+      <c r="K17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="M17" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="N17" s="5" t="s">
+      <c r="M17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="N17" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="O17" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P17" s="5" t="s">
+      <c r="O17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P17" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="Q17" s="5" t="s">
+      <c r="Q17" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="R17" s="2"/>
+      <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="B18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="M18" s="4" t="s">
+      <c r="L18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="N18" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="O18" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="P18" s="4" t="s">
+      <c r="N18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="P18" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="Q18" s="4" t="s">
+      <c r="Q18" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="R18" s="3"/>
+      <c r="R18" s="2"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="B19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="5" t="s">
+      <c r="E19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J19" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="L19" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="M19" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="2"/>
+      <c r="M19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="L20" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="M20" s="4" t="s">
+      <c r="M20" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="N20" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="O20" s="4" t="s">
+      <c r="N20" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O20" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="P20" s="4" t="s">
+      <c r="P20" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="Q20" s="4" t="s">
+      <c r="Q20" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="R20" s="3"/>
+      <c r="R20" s="2"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="5" t="s">
+      <c r="C21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H21" s="5" t="s">
+      <c r="G21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="J21" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="K21" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5" t="s">
+      <c r="L21" s="4"/>
+      <c r="M21" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="2"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H22" s="4" t="s">
+      <c r="G22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="J22" s="4" t="s">
+      <c r="I22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J22" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L22" s="4" t="s">
+      <c r="L22" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="M22" s="4" t="s">
+      <c r="M22" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="N22" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="O22" s="4" t="s">
+      <c r="N22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O22" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P22" s="4" t="s">
+      <c r="P22" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="Q22" s="4" t="s">
+      <c r="Q22" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="R22" s="3"/>
+      <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="G23" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5" t="s">
+      <c r="G23" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="K23" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="2"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="1"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="2"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5" t="s">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="O25" s="5" t="s">
+      <c r="O25" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="2"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="1"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="R26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="R26" s="2"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5" t="s">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="O27" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P27" s="5" t="s">
+      <c r="O27" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P27" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="2"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="1"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="L28" s="4" t="s">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L28" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4" t="s">
+      <c r="M28" s="3"/>
+      <c r="N28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="O28" s="4" t="s">
+      <c r="O28" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="P28" s="4" t="s">
+      <c r="P28" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="Q28" s="4" t="s">
+      <c r="Q28" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="R28" s="3"/>
+      <c r="R28" s="2"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5" t="s">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5" t="s">
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="2"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="1"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4" t="s">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="N30" s="4" t="s">
+      <c r="N30" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="O30" s="4" t="s">
+      <c r="O30" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="P30" s="4" t="s">
+      <c r="P30" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="2"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D31" s="5" t="s">
+      <c r="C31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H31" s="5" t="s">
+      <c r="E31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H31" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I31" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="K31" s="5" t="s">
+      <c r="I31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K31" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5" t="s">
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="R31" s="2"/>
+      <c r="R31" s="1"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4" t="s">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="P32" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q32" s="4" t="s">
+      <c r="P32" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q32" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="R32" s="3"/>
+      <c r="R32" s="2"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5" t="s">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F33" s="5" t="s">
+      <c r="D33" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G33" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="H33" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="I33" s="5" t="s">
+      <c r="I33" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="J33" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5" t="s">
+      <c r="J33" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="R33" s="2"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="R33" s="1"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4" t="s">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="Q34" s="4" t="s">
+      <c r="Q34" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="R34" s="3"/>
+      <c r="R34" s="2"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="5"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
-      <c r="R35" s="2"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="1"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6141,67 +6114,67 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" t="s">
         <v>214</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>215</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>216</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>217</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>218</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>219</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>220</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>221</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>222</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>223</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>224</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>225</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>226</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>227</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>228</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>229</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>230</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>231</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>232</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>233</v>
-      </c>
-      <c r="U1" t="s">
-        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadidos 125 y 250 hasta el año 2003
</commit_message>
<xml_diff>
--- a/Excels/data/2004.xlsx
+++ b/Excels/data/2004.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73EE76A4-4622-4F47-988E-650D4EFDD700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF84D90-BC9D-4BEC-80D8-F21814366571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="1" activeTab="4" xr2:uid="{5FACFDE8-0E5D-450C-9997-A9F216FA1A6F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{5FACFDE8-0E5D-450C-9997-A9F216FA1A6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="237">
   <si>
     <t>Round</t>
   </si>
@@ -853,6 +853,12 @@
   </si>
   <si>
     <t>rider</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>motogp</t>
   </si>
 </sst>
 </file>
@@ -924,17 +930,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1033,8 +1043,8 @@
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatosExternos_3" backgroundRefresh="0" connectionId="11" xr16:uid="{90F88823-2D05-4511-9E3E-E1F4740B48B0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="8">
-    <queryTableFields count="7">
+  <queryTableRefresh nextId="9" unboundColumnsRight="1">
+    <queryTableFields count="8">
       <queryTableField id="1" name="Team" tableColumnId="1"/>
       <queryTableField id="2" name="Constructor" tableColumnId="2"/>
       <queryTableField id="3" name="Motorcycle" tableColumnId="3"/>
@@ -1042,6 +1052,7 @@
       <queryTableField id="5" name="No." tableColumnId="5"/>
       <queryTableField id="6" name="Rider" tableColumnId="6"/>
       <queryTableField id="7" name="Rounds" tableColumnId="7"/>
+      <queryTableField id="8" dataBound="0" tableColumnId="8"/>
     </queryTableFields>
   </queryTableRefresh>
   <extLst>
@@ -1092,9 +1103,9 @@
   <autoFilter ref="A1:D17" xr:uid="{9CC30863-27A7-460B-91DB-4F2B3FE00919}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A8239CEB-8E16-48C8-B08C-CFBB188728E6}" uniqueName="1" name="Round" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{D7EFC2CF-C8AC-41D1-B4C0-6AC84AF9BAD0}" uniqueName="2" name="Date" queryTableFieldId="2" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{E2263DA5-CD7E-43F3-A7FC-4A9DB5E0F919}" uniqueName="3" name="Grand Prix" queryTableFieldId="3" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{9F4F59C1-B981-4BC1-BB91-9135C695CB7D}" uniqueName="4" name="Circuit" queryTableFieldId="4" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{D7EFC2CF-C8AC-41D1-B4C0-6AC84AF9BAD0}" uniqueName="2" name="Date" queryTableFieldId="2" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{E2263DA5-CD7E-43F3-A7FC-4A9DB5E0F919}" uniqueName="3" name="Grand Prix" queryTableFieldId="3" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{9F4F59C1-B981-4BC1-BB91-9135C695CB7D}" uniqueName="4" name="Circuit" queryTableFieldId="4" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1131,16 +1142,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2877D334-4B77-4545-9145-95F4CE2CAED9}" name="Table_2__2" displayName="Table_2__2" ref="A1:G38" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G38" xr:uid="{2877D334-4B77-4545-9145-95F4CE2CAED9}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8C4EB136-5FC9-46C8-B0ED-46E0E78443B8}" uniqueName="1" name="Team" queryTableFieldId="1" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{F59223B6-7A34-4A36-AED3-1F66BCA89A14}" uniqueName="2" name="Constructor" queryTableFieldId="2" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{2FE2C583-1870-48B2-B408-75622E985780}" uniqueName="3" name="Motorcycle" queryTableFieldId="3" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{CA5F9221-D928-4265-8A26-3FB626805EB9}" uniqueName="4" name="Tyres" queryTableFieldId="4" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{AADBFAC4-9813-47E0-9ECF-2162C8A9EE53}" uniqueName="5" name="No." queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{B8E77ADC-39B4-42DA-85DE-A9C678DA6818}" uniqueName="6" name="Rider" queryTableFieldId="6" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{57AF8B8B-25F3-43EA-982F-17C3934ADE3F}" uniqueName="7" name="Rounds" queryTableFieldId="7" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2877D334-4B77-4545-9145-95F4CE2CAED9}" name="Table_2__2" displayName="Table_2__2" ref="A1:H38" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:H38" xr:uid="{2877D334-4B77-4545-9145-95F4CE2CAED9}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{8C4EB136-5FC9-46C8-B0ED-46E0E78443B8}" uniqueName="1" name="Team" queryTableFieldId="1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F59223B6-7A34-4A36-AED3-1F66BCA89A14}" uniqueName="2" name="Constructor" queryTableFieldId="2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{2FE2C583-1870-48B2-B408-75622E985780}" uniqueName="3" name="Motorcycle" queryTableFieldId="3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{CA5F9221-D928-4265-8A26-3FB626805EB9}" uniqueName="4" name="Tyres" queryTableFieldId="4" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{AADBFAC4-9813-47E0-9ECF-2162C8A9EE53}" uniqueName="5" name="No." queryTableFieldId="5" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{B8E77ADC-39B4-42DA-85DE-A9C678DA6818}" uniqueName="6" name="Rider" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{57AF8B8B-25F3-43EA-982F-17C3934ADE3F}" uniqueName="7" name="Rounds" queryTableFieldId="7" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{CEF07E70-1598-4EA8-B658-5760299944C4}" uniqueName="8" name="class" queryTableFieldId="8" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1749,7 +1761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DCEEADA-21DE-4E09-A46D-C942026BBB0D}">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -3588,10 +3600,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79ED2529-CCA3-4F4F-A698-BE65E13E91F5}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3605,7 +3617,7 @@
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -3627,8 +3639,11 @@
       <c r="G1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -3650,8 +3665,11 @@
       <c r="G2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>128</v>
       </c>
@@ -3673,8 +3691,11 @@
       <c r="G3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -3696,8 +3717,11 @@
       <c r="G4" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -3719,8 +3743,11 @@
       <c r="G5" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -3742,8 +3769,11 @@
       <c r="G6" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -3765,8 +3795,11 @@
       <c r="G7" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>109</v>
       </c>
@@ -3788,8 +3821,11 @@
       <c r="G8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>109</v>
       </c>
@@ -3811,8 +3847,11 @@
       <c r="G9" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>135</v>
       </c>
@@ -3834,8 +3873,11 @@
       <c r="G10" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>135</v>
       </c>
@@ -3857,8 +3899,11 @@
       <c r="G11" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -3880,8 +3925,11 @@
       <c r="G12" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -3903,8 +3951,11 @@
       <c r="G13" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>135</v>
       </c>
@@ -3926,8 +3977,11 @@
       <c r="G14" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>91</v>
       </c>
@@ -3949,8 +4003,11 @@
       <c r="G15" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -3972,8 +4029,11 @@
       <c r="G16" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>155</v>
       </c>
@@ -3995,8 +4055,11 @@
       <c r="G17" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -4018,8 +4081,11 @@
       <c r="G18" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>82</v>
       </c>
@@ -4041,8 +4107,11 @@
       <c r="G19" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -4064,8 +4133,11 @@
       <c r="G20" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -4087,8 +4159,11 @@
       <c r="G21" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>106</v>
       </c>
@@ -4110,8 +4185,11 @@
       <c r="G22" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>106</v>
       </c>
@@ -4133,8 +4211,11 @@
       <c r="G23" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>140</v>
       </c>
@@ -4156,8 +4237,11 @@
       <c r="G24" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>140</v>
       </c>
@@ -4179,8 +4263,11 @@
       <c r="G25" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>196</v>
       </c>
@@ -4202,8 +4289,11 @@
       <c r="G26" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>196</v>
       </c>
@@ -4225,8 +4315,11 @@
       <c r="G27" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>196</v>
       </c>
@@ -4248,8 +4341,11 @@
       <c r="G28" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>121</v>
       </c>
@@ -4271,8 +4367,11 @@
       <c r="G29" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>121</v>
       </c>
@@ -4294,8 +4393,11 @@
       <c r="G30" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>121</v>
       </c>
@@ -4317,8 +4419,11 @@
       <c r="G31" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -4340,8 +4445,11 @@
       <c r="G32" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>121</v>
       </c>
@@ -4363,8 +4471,11 @@
       <c r="G33" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -4386,8 +4497,11 @@
       <c r="G34" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>75</v>
       </c>
@@ -4409,8 +4523,11 @@
       <c r="G35" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>112</v>
       </c>
@@ -4432,8 +4549,11 @@
       <c r="G36" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>112</v>
       </c>
@@ -4455,6 +4575,12 @@
       <c r="G37" t="s">
         <v>169</v>
       </c>
+      <c r="H37" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4468,7 +4594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34FD487F-3DE1-4D7E-AC38-49F580DAF036}">
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:Z1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
normalizado el nombre de Raffaele de Rosa en todos los excels
</commit_message>
<xml_diff>
--- a/Excels/data/2004.xlsx
+++ b/Excels/data/2004.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2EEE26-9C4B-450D-9D7B-2D5D2D1E820F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1780F023-98D1-45F1-9538-7CF21C29CA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="18075" windowHeight="12255" tabRatio="766" firstSheet="1" activeTab="4" xr2:uid="{5FACFDE8-0E5D-450C-9997-A9F216FA1A6F}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="18075" windowHeight="12255" tabRatio="766" firstSheet="4" activeTab="10" xr2:uid="{5FACFDE8-0E5D-450C-9997-A9F216FA1A6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -222,7 +222,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5412" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5412" uniqueCount="580">
   <si>
     <t>Round</t>
   </si>
@@ -1959,6 +1959,9 @@
   </si>
   <si>
     <t>125cc</t>
+  </si>
+  <si>
+    <t>Raffaele de Rosa</t>
   </si>
 </sst>
 </file>
@@ -2959,7 +2962,7 @@
   <dimension ref="A1:H89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3328,7 +3331,7 @@
         <v>377</v>
       </c>
       <c r="F14" t="s">
-        <v>361</v>
+        <v>579</v>
       </c>
       <c r="G14" t="s">
         <v>93</v>
@@ -5287,8 +5290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11263162-ECE2-4C64-AEBE-3AED40C34CB8}">
   <dimension ref="A1:AA89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7749,7 +7752,7 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>361</v>
+        <v>579</v>
       </c>
       <c r="B55" t="s">
         <v>578</v>
@@ -11752,7 +11755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34FD487F-3DE1-4D7E-AC38-49F580DAF036}">
   <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>